<commit_message>
responses rates nlo 2
</commit_message>
<xml_diff>
--- a/data/9.lookups/lkp_clean_sections_nlo_part_II.xlsx
+++ b/data/9.lookups/lkp_clean_sections_nlo_part_II.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositaries\1.work\IAEA3\data\9.lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7BDC425-E82B-4E3D-82C2-2B2E72AF1065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED64BA4E-D01B-4D1B-96E7-EFFCA869A5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14028" yWindow="19344" windowWidth="22752" windowHeight="14748" xr2:uid="{B96A5D1D-0978-4BF8-AC3B-F7ACF8A0D866}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{B96A5D1D-0978-4BF8-AC3B-F7ACF8A0D866}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="themes" sheetId="1" r:id="rId1"/>
+    <sheet name="foas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
   <si>
     <t>theme</t>
   </si>
@@ -66,6 +67,9 @@
   </si>
   <si>
     <t>ends</t>
+  </si>
+  <si>
+    <t>foa_id</t>
   </si>
 </sst>
 </file>
@@ -81,15 +85,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,12 +107,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,12 +448,12 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -439,7 +467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -453,7 +481,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -467,7 +495,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -478,10 +506,10 @@
         <v>54</v>
       </c>
       <c r="D4">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -495,7 +523,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -509,7 +537,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -520,6 +548,310 @@
         <v>75</v>
       </c>
       <c r="D7">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EEDD90-E0AD-4CBC-BEAB-56EED9AE375A}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>40</v>
+      </c>
+      <c r="E8" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>49</v>
+      </c>
+      <c r="E9" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>59</v>
+      </c>
+      <c r="E12" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>62</v>
+      </c>
+      <c r="E13" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>67</v>
+      </c>
+      <c r="E14" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>71</v>
+      </c>
+      <c r="E15" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>75</v>
+      </c>
+      <c r="E16" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>79</v>
+      </c>
+      <c r="E17" s="3">
         <v>83</v>
       </c>
     </row>

</xml_diff>